<commit_message>
adding test files, including catchKey.py with list routine
</commit_message>
<xml_diff>
--- a/isbns.xlsx
+++ b/isbns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/846f05906f3c79a7/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/846f05906f3c79a7/Documents/isbn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{436CE455-149F-4EDE-8B84-58255F586BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{305F2484-0CF8-4E6E-81A0-45BBFFEF8862}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{436CE455-149F-4EDE-8B84-58255F586BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAEE7790-9934-454C-A5D5-EAA6BBBD9381}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{766DABD9-B856-4B8A-AB36-22B89BFE4160}"/>
+    <workbookView xWindow="45795" yWindow="3225" windowWidth="22485" windowHeight="14535" xr2:uid="{766DABD9-B856-4B8A-AB36-22B89BFE4160}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +59,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,10 +91,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,35 +413,45 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>9780358344582</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>9781416571728</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>9781491927571</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>9781449357016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>